<commit_message>
carga de tareas en GitHub Prject
</commit_message>
<xml_diff>
--- a/paperwork/Tareas Sprint1.xlsx
+++ b/paperwork/Tareas Sprint1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\ParentLink\ParentLink\paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B405CD6-1349-41C8-AAD2-8C880EE31E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91332283-27A9-4CA0-82EC-0BE54C9CBCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>Implementar los componentes básicos de la HOME en React y configuren el enrutamiento con React Router para futuras pantallas. Esto asegura una base sólida.</t>
   </si>
   <si>
-    <t xml:space="preserve">Desarrollo de la API-REST con los endpoints CRUD </t>
-  </si>
-  <si>
     <t>Definición del PMV (prod. mín. viable)</t>
   </si>
   <si>
@@ -258,6 +255,9 @@
   </si>
   <si>
     <t>Montar tareas en GibHub Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollo Basico de la API-REST con los endpoints CRUD </t>
   </si>
 </sst>
 </file>
@@ -330,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -363,9 +363,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -375,9 +372,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -385,10 +379,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,8 +606,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.61328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -743,10 +740,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>7</v>
@@ -755,10 +752,10 @@
         <v>45664</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -786,10 +783,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
@@ -827,13 +824,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="8">
         <v>45666</v>
@@ -866,10 +863,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>7</v>
@@ -878,7 +875,7 @@
         <v>45666</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -907,13 +904,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="E8" s="8">
         <v>45666</v>
@@ -974,17 +971,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1013,17 +1010,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1052,10 +1049,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>7</v>
@@ -1068,13 +1065,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="9">
         <v>45666</v>
@@ -1087,13 +1084,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="11">
         <v>45664</v>
@@ -1106,7 +1103,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>6</v>
@@ -6055,37 +6052,37 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.3046875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.3046875" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.4609375" customWidth="1"/>
     <col min="4" max="4" width="12.61328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
       </c>
       <c r="C2" s="9">
         <v>45667</v>
@@ -6095,9 +6092,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
+      <c r="A3" s="21"/>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="9">
         <v>45670</v>
@@ -6107,9 +6104,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="37.299999999999997" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="9">
         <v>45670</v>
@@ -6119,9 +6116,9 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="21"/>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="9">
         <v>45670</v>
@@ -6131,9 +6128,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+      <c r="A6" s="21"/>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="9">
         <v>45670</v>
@@ -6143,9 +6140,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="21"/>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="9">
         <v>45670</v>
@@ -6155,9 +6152,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
+      <c r="A8" s="21"/>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="9">
         <v>45670</v>
@@ -6167,9 +6164,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="21"/>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="9">
         <v>45670</v>
@@ -6179,9 +6176,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="A10" s="21"/>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="9">
         <v>45670</v>
@@ -6191,43 +6188,43 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>62</v>
+      <c r="A11" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="37.299999999999997" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>57</v>
+      <c r="A12" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="C12" s="9">
         <v>45670</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="37.299999999999997" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="9">
         <v>45670</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="37.299999999999997" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="9">
         <v>45670</v>
@@ -6237,21 +6234,21 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="49.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="9">
         <v>45670</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="24.9" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="9">
         <v>45670</v>
@@ -6261,9 +6258,9 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="37.299999999999997" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="9">
         <v>45670</v>
@@ -6273,13 +6270,13 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="23">
+      <c r="C18" s="20">
         <v>45670</v>
       </c>
       <c r="D18" s="13" t="s">
@@ -6291,11 +6288,11 @@
       <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" ht="24.9" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>52</v>
+      <c r="A20" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="C20" s="9">
         <v>45670</v>
@@ -6305,76 +6302,76 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="15" t="s">
-        <v>67</v>
+      <c r="A21" s="21"/>
+      <c r="B21" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="15" t="s">
-        <v>68</v>
+      <c r="A22" s="21"/>
+      <c r="B22" s="14" t="s">
+        <v>67</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="14"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="14"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="14"/>
+      <c r="B26" s="12"/>
     </row>
     <row r="27" spans="1:4" ht="24.9" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="15" t="s">
         <v>54</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="24.9" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
-      <c r="B28" s="14" t="s">
-        <v>53</v>
+      <c r="B28" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="24.9" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
-      <c r="B29" s="14" t="s">
-        <v>56</v>
+      <c r="B29" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="31" spans="1:4" ht="62.15" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>